<commit_message>
hardware, ordering: update 0_ramn orders BOM to correct C11 C12 C21 C22 C31 C32 C41 C42 to 1206 part
</commit_message>
<xml_diff>
--- a/hardware/orders/0_ramn/bom.xlsx
+++ b/hardware/orders/0_ramn/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\563554\src\RAMN\hardware\orders\0_ramn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A21D8E-77C7-4865-A7E6-AC7950B6D82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C02FDB-B58E-4666-AB63-D52B11D990CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19590" yWindow="-20985" windowWidth="39855" windowHeight="20985" xr2:uid="{122D935A-FDA2-4194-8296-BF46E66E2E5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{122D935A-FDA2-4194-8296-BF46E66E2E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>Item #</t>
   </si>
@@ -161,12 +161,6 @@
     <t xml:space="preserve">C11 C12 C21 C22 C31 C32 C41 C42 </t>
   </si>
   <si>
-    <t>CAP CER 1UF 25V X7R 0805</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
     <t>C3 C4 C8 C9 C10 C13 C14 C18 C19 C20 C23 C24 C28 C29 C30 C33 C34 C38 C39 C40 C43</t>
   </si>
   <si>
@@ -343,12 +337,13 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>GCM21BR71E105KA56L</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>The package in gerber is 1206, the correct part number is CL31B105KAHNNNE</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V X7R 1206</t>
+  </si>
+  <si>
+    <t>GCM31CL81H105KA55L</t>
   </si>
 </sst>
 </file>
@@ -893,7 +888,7 @@
   <dimension ref="A2:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -989,7 +984,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30.75" thickBot="1">
@@ -1022,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="90.75" thickBot="1">
+    <row r="8" spans="1:11" ht="45.75" thickBot="1">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -1039,10 +1034,10 @@
         <v>88</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>9</v>
@@ -1051,16 +1046,14 @@
       <c r="J8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="16" t="s">
-        <v>89</v>
-      </c>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" ht="105.75" thickBot="1">
       <c r="A9" s="4">
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7">
         <v>21</v>
@@ -1069,10 +1062,10 @@
         <v>26</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>11</v>
@@ -1090,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="7">
         <v>8</v>
@@ -1099,10 +1092,10 @@
         <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>11</v>
@@ -1120,7 +1113,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7">
         <v>4</v>
@@ -1129,10 +1122,10 @@
         <v>26</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" s="8">
         <v>1206</v>
@@ -1150,16 +1143,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7">
         <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -1180,19 +1173,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7">
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>11</v>
@@ -1210,19 +1203,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="7">
         <v>4</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>11</v>
@@ -1240,19 +1233,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="10">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>11</v>
@@ -1270,19 +1263,19 @@
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>9</v>
@@ -1300,19 +1293,19 @@
         <v>11</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="10">
         <v>1</v>
       </c>
       <c r="D17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>15</v>
@@ -1330,19 +1323,19 @@
         <v>12</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10">
         <v>4</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>17</v>
@@ -1360,7 +1353,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="10">
         <v>10</v>
@@ -1390,22 +1383,22 @@
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" s="7">
         <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="G20" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>9</v>
@@ -1420,7 +1413,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="7">
         <v>4</v>
@@ -1429,13 +1422,13 @@
         <v>22</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>9</v>
@@ -1450,22 +1443,22 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="7">
         <v>4</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="G22" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>9</v>
@@ -1480,19 +1473,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="7">
         <v>4</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>23</v>
@@ -1510,22 +1503,22 @@
         <v>18</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" s="7">
         <v>4</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
hardware, orders: fix 0_ramn expansion sockets: do not mark DNP
</commit_message>
<xml_diff>
--- a/hardware/orders/0_ramn/bom.xlsx
+++ b/hardware/orders/0_ramn/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\563554\src\RAMN\hardware\orders\0_ramn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C02FDB-B58E-4666-AB63-D52B11D990CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA426B9-FCF0-40C1-9496-1095EEAFF725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{122D935A-FDA2-4194-8296-BF46E66E2E5D}"/>
+    <workbookView xWindow="17205" yWindow="-21600" windowWidth="20040" windowHeight="20985" xr2:uid="{122D935A-FDA2-4194-8296-BF46E66E2E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="2" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -570,6 +570,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,7 +897,7 @@
   <dimension ref="A2:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,34 +1328,34 @@
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A18" s="14">
+      <c r="A18" s="4">
         <v>12</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="20">
         <v>4</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="12"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="60.75" thickBot="1">
       <c r="A19" s="4">

</xml_diff>